<commit_message>
adding community benefit project
</commit_message>
<xml_diff>
--- a/2018/cvstimeline-20181012/cvstimeline-20181012.xlsx
+++ b/2018/cvstimeline-20181012/cvstimeline-20181012.xlsx
@@ -17,22 +17,22 @@
     <t>state</t>
   </si>
   <si>
+    <t>something</t>
+  </si>
+  <si>
     <t>key</t>
   </si>
   <si>
-    <t>something</t>
+    <t>another_thing</t>
   </si>
   <si>
     <t>value</t>
   </si>
   <si>
-    <t>another_thing</t>
+    <t>Alabama</t>
   </si>
   <si>
     <t>headline</t>
-  </si>
-  <si>
-    <t>Alabama</t>
   </si>
   <si>
     <t>2</t>
@@ -59,9 +59,6 @@
     <t>1912</t>
   </si>
   <si>
-    <t>subhed</t>
-  </si>
-  <si>
     <t>Arkansas</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>1836</t>
+  </si>
+  <si>
+    <t>subhed</t>
   </si>
   <si>
     <t>California</t>
@@ -135,10 +135,10 @@
       <b/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="14.0"/>
     </font>
     <font/>
   </fonts>
@@ -169,29 +169,29 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -226,42 +226,42 @@
   </cols>
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
     <row r="2" ht="33.0" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
+      <c r="A2" s="7" t="s">
+        <v>6</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -288,8 +288,8 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" ht="33.0" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>15</v>
+      <c r="A3" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="9"/>
@@ -318,10 +318,10 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" ht="33.0" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -348,10 +348,10 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" ht="33.0" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="9"/>
@@ -380,10 +380,10 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" ht="33.0" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="9"/>
@@ -713,39 +713,39 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>6</v>
+      <c r="A2" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>7</v>
@@ -755,7 +755,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -766,7 +766,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -777,18 +777,18 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -799,7 +799,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -810,7 +810,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="8" t="s">

</xml_diff>